<commit_message>
Added FLOPS for each model. FLOP calculation using 'thop' library
</commit_message>
<xml_diff>
--- a/eval_results_combined.xlsx
+++ b/eval_results_combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Thesis_Git\Complex-YOLOv3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F703E4FA-497F-474A-B9C1-90D25689E219}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF5CBE1-13E3-49BB-9C35-D3B3F587D0A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="14760" windowHeight="11910" xr2:uid="{33803897-E998-4B3C-BE2B-F40B7580F66B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{33803897-E998-4B3C-BE2B-F40B7580F66B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>Model</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>FPS</t>
+  </si>
+  <si>
+    <t>FLOPS (G)</t>
   </si>
 </sst>
 </file>
@@ -164,16 +167,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,846 +492,949 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DCF2CE-8D1A-4C95-B84A-DAFE67D6BD13}">
-  <dimension ref="C2:I39"/>
+  <dimension ref="C2:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C2" s="7" t="s">
+    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="4"/>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="1">
+        <v>70</v>
+      </c>
+      <c r="E5" s="1">
         <v>62.5</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>93.59</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>70.44</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>86.39</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>658.12</v>
       </c>
-      <c r="I5" s="1">
-        <f>ROUND((1/H5)*1000,2)</f>
+      <c r="J5" s="1">
+        <f>ROUND((1/I5)*1000,2)</f>
         <v>1.52</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="1">
+        <v>13.99</v>
+      </c>
+      <c r="E6" s="1">
         <v>12.5</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>92.31</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>67.88</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>86.41</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>288.68</v>
       </c>
-      <c r="I6" s="1">
-        <f t="shared" ref="I6:I19" si="0">ROUND((1/H6)*1000,2)</f>
+      <c r="J6" s="1">
+        <f t="shared" ref="J6:J19" si="0">ROUND((1/I6)*1000,2)</f>
         <v>3.46</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="1">
+        <v>21.76</v>
+      </c>
+      <c r="E7" s="1">
         <v>24.2</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>89.93</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>72.7</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>79.41</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>297.18</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <f t="shared" si="0"/>
         <v>3.36</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="1">
+        <v>13.67</v>
+      </c>
+      <c r="E8" s="1">
         <v>16.03</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>75.95</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>54.74</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>74.239999999999995</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>271.89</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <f t="shared" si="0"/>
         <v>3.68</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="1">
+        <v>12.21</v>
+      </c>
+      <c r="E9" s="1">
         <v>15.61</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>85.07</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>48.89</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>56.21</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>290.02</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <f t="shared" si="0"/>
         <v>3.45</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="1">
+        <v>11.07</v>
+      </c>
+      <c r="E10" s="1">
         <v>13.91</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>91.56</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>59.76</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>80.98</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>220.02</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <f t="shared" si="0"/>
         <v>4.55</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="1">
+        <v>7.24</v>
+      </c>
+      <c r="E11" s="1">
         <v>8.4700000000000006</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>90.07</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>59.39</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <v>78.17</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>189.2</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <f t="shared" si="0"/>
         <v>5.29</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="1">
+        <v>4.67</v>
+      </c>
+      <c r="E12" s="1">
         <v>5.7</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>87.33</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <v>61.99</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>63.59</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>143.62</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <f t="shared" si="0"/>
         <v>6.96</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="1">
+        <v>6.39</v>
+      </c>
+      <c r="E13" s="1">
         <v>7.79</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>85.7</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="1">
         <v>59.76</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>77.8</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>163.30000000000001</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <f t="shared" si="0"/>
         <v>6.12</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="1">
+        <v>6.39</v>
+      </c>
+      <c r="E14" s="1">
         <v>7.79</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>83.82</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>51.95</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>62.35</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>185.37</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <f t="shared" si="0"/>
         <v>5.39</v>
       </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="1">
+        <v>20.7</v>
+      </c>
+      <c r="E15" s="1">
         <v>22.13</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>92.59</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>70.28</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>83.09</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>272.52</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <f t="shared" si="0"/>
         <v>3.67</v>
       </c>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="1">
+        <v>29.58</v>
+      </c>
+      <c r="E16" s="1">
         <v>22.12</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>91.35</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>68.47</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <v>83.39</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>422.62</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <f t="shared" si="0"/>
         <v>2.37</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="E17" s="1">
         <v>5.64</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>85.07</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>66.150000000000006</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <v>79.92</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>308.04000000000002</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17" s="1">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="1">
+        <v>22.34</v>
+      </c>
+      <c r="E18" s="1">
         <v>21.46</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>92.77</v>
       </c>
-      <c r="F18" s="3">
+      <c r="G18" s="3">
         <v>70.349999999999994</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <v>76.8</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>289.95</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J18" s="1">
         <f t="shared" si="0"/>
         <v>3.45</v>
       </c>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
+        <v>8.76</v>
+      </c>
+      <c r="E19" s="2">
         <v>4.97</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>91.92</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>62.41</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>78.09</v>
       </c>
-      <c r="H19" s="3">
+      <c r="I19" s="3">
         <v>182.67</v>
       </c>
-      <c r="I19" s="1">
+      <c r="J19" s="1">
         <f t="shared" si="0"/>
         <v>5.47</v>
       </c>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C22" s="7" t="s">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="4" t="s">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="F23" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="6"/>
+      <c r="I23" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="J23" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C24" s="4"/>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="7"/>
+      <c r="F24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="1">
+        <v>70</v>
+      </c>
+      <c r="E25" s="1">
         <v>62.5</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <v>93.59</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>70.44</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <v>86.39</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <v>46.56</v>
       </c>
-      <c r="I25" s="1">
-        <f t="shared" ref="I25:I39" si="1">ROUND((1/H25)*1000,2)</f>
+      <c r="J25" s="1">
+        <f t="shared" ref="J25:J39" si="1">ROUND((1/I25)*1000,2)</f>
         <v>21.48</v>
       </c>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D26" s="1">
+        <v>13.99</v>
+      </c>
+      <c r="E26" s="1">
         <v>12.5</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <v>92.31</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="1">
         <v>67.88</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <v>86.41</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="1">
         <v>34.64</v>
       </c>
-      <c r="I26" s="1">
+      <c r="J26" s="1">
         <f t="shared" si="1"/>
         <v>28.87</v>
       </c>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="1">
+        <v>21.76</v>
+      </c>
+      <c r="E27" s="1">
         <v>24.2</v>
       </c>
-      <c r="E27" s="1">
+      <c r="F27" s="1">
         <v>89.93</v>
       </c>
-      <c r="F27" s="1">
+      <c r="G27" s="1">
         <v>72.7</v>
       </c>
-      <c r="G27" s="1">
+      <c r="H27" s="1">
         <v>79.41</v>
       </c>
-      <c r="H27" s="1">
+      <c r="I27" s="1">
         <v>45.02</v>
       </c>
-      <c r="I27" s="1">
+      <c r="J27" s="1">
         <f t="shared" si="1"/>
         <v>22.21</v>
       </c>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="1">
+        <v>13.67</v>
+      </c>
+      <c r="E28" s="1">
         <v>16.03</v>
       </c>
-      <c r="E28" s="1">
+      <c r="F28" s="1">
         <v>75.95</v>
       </c>
-      <c r="F28" s="1">
+      <c r="G28" s="1">
         <v>54.74</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <v>74.239999999999995</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>37.57</v>
       </c>
-      <c r="I28" s="1">
+      <c r="J28" s="1">
         <f t="shared" si="1"/>
         <v>26.62</v>
       </c>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D29" s="1">
+        <v>12.21</v>
+      </c>
+      <c r="E29" s="1">
         <v>15.61</v>
       </c>
-      <c r="E29" s="1">
+      <c r="F29" s="1">
         <v>85.07</v>
       </c>
-      <c r="F29" s="1">
+      <c r="G29" s="1">
         <v>48.89</v>
       </c>
-      <c r="G29" s="1">
+      <c r="H29" s="1">
         <v>56.21</v>
       </c>
-      <c r="H29" s="1">
+      <c r="I29" s="1">
         <v>64.94</v>
       </c>
-      <c r="I29" s="1">
+      <c r="J29" s="1">
         <f t="shared" si="1"/>
         <v>15.4</v>
       </c>
     </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="1">
+        <v>11.07</v>
+      </c>
+      <c r="E30" s="1">
         <v>13.91</v>
       </c>
-      <c r="E30" s="1">
+      <c r="F30" s="1">
         <v>91.56</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <v>59.76</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
         <v>80.98</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>38.31</v>
       </c>
-      <c r="I30" s="1">
+      <c r="J30" s="1">
         <f t="shared" si="1"/>
         <v>26.1</v>
       </c>
     </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="1">
+        <v>7.24</v>
+      </c>
+      <c r="E31" s="1">
         <v>8.4700000000000006</v>
       </c>
-      <c r="E31" s="1">
+      <c r="F31" s="1">
         <v>90.07</v>
       </c>
-      <c r="F31" s="1">
+      <c r="G31" s="1">
         <v>59.39</v>
       </c>
-      <c r="G31" s="1">
+      <c r="H31" s="1">
         <v>78.17</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <v>41.37</v>
       </c>
-      <c r="I31" s="1">
+      <c r="J31" s="1">
         <f t="shared" si="1"/>
         <v>24.17</v>
       </c>
     </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C32" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="1">
+        <v>4.67</v>
+      </c>
+      <c r="E32" s="1">
         <v>5.7</v>
       </c>
-      <c r="E32" s="1">
+      <c r="F32" s="1">
         <v>87.33</v>
       </c>
-      <c r="F32" s="1">
+      <c r="G32" s="1">
         <v>61.99</v>
       </c>
-      <c r="G32" s="1">
+      <c r="H32" s="1">
         <v>63.59</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <v>37.24</v>
       </c>
-      <c r="I32" s="1">
+      <c r="J32" s="1">
         <f t="shared" si="1"/>
         <v>26.85</v>
       </c>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D33" s="1">
+        <v>6.39</v>
+      </c>
+      <c r="E33" s="1">
         <v>7.79</v>
       </c>
-      <c r="E33" s="1">
+      <c r="F33" s="1">
         <v>85.7</v>
       </c>
-      <c r="F33" s="1">
+      <c r="G33" s="1">
         <v>59.76</v>
       </c>
-      <c r="G33" s="1">
+      <c r="H33" s="1">
         <v>77.8</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <v>35.6</v>
       </c>
-      <c r="I33" s="1">
+      <c r="J33" s="1">
         <f t="shared" si="1"/>
         <v>28.09</v>
       </c>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D34" s="1">
+        <v>6.39</v>
+      </c>
+      <c r="E34" s="1">
         <v>7.79</v>
       </c>
-      <c r="E34" s="1">
+      <c r="F34" s="1">
         <v>83.82</v>
       </c>
-      <c r="F34" s="1">
+      <c r="G34" s="1">
         <v>51.95</v>
       </c>
-      <c r="G34" s="1">
+      <c r="H34" s="1">
         <v>62.35</v>
       </c>
-      <c r="H34" s="1">
+      <c r="I34" s="1">
         <v>50.77</v>
       </c>
-      <c r="I34" s="1">
+      <c r="J34" s="1">
         <f t="shared" si="1"/>
         <v>19.7</v>
       </c>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D35" s="1">
+        <v>20.7</v>
+      </c>
+      <c r="E35" s="1">
         <v>22.13</v>
       </c>
-      <c r="E35" s="1">
+      <c r="F35" s="1">
         <v>92.59</v>
       </c>
-      <c r="F35" s="1">
+      <c r="G35" s="1">
         <v>70.28</v>
       </c>
-      <c r="G35" s="1">
+      <c r="H35" s="1">
         <v>83.09</v>
       </c>
-      <c r="H35" s="1">
+      <c r="I35" s="1">
         <v>35.75</v>
       </c>
-      <c r="I35" s="1">
+      <c r="J35" s="1">
         <f t="shared" si="1"/>
         <v>27.97</v>
       </c>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D36" s="1">
+        <v>29.58</v>
+      </c>
+      <c r="E36" s="1">
         <v>22.12</v>
       </c>
-      <c r="E36" s="1">
+      <c r="F36" s="1">
         <v>91.35</v>
       </c>
-      <c r="F36" s="1">
+      <c r="G36" s="1">
         <v>68.47</v>
       </c>
-      <c r="G36" s="1">
+      <c r="H36" s="1">
         <v>83.39</v>
       </c>
-      <c r="H36" s="1">
+      <c r="I36" s="1">
         <v>37.5</v>
       </c>
-      <c r="I36" s="1">
+      <c r="J36" s="1">
         <f t="shared" si="1"/>
         <v>26.67</v>
       </c>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D37" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="E37" s="1">
         <v>5.64</v>
       </c>
-      <c r="E37" s="1">
+      <c r="F37" s="1">
         <v>85.07</v>
       </c>
-      <c r="F37" s="1">
+      <c r="G37" s="1">
         <v>66.150000000000006</v>
       </c>
-      <c r="G37" s="1">
+      <c r="H37" s="1">
         <v>79.92</v>
       </c>
-      <c r="H37" s="1">
+      <c r="I37" s="1">
         <v>40.19</v>
       </c>
-      <c r="I37" s="1">
+      <c r="J37" s="1">
         <f t="shared" si="1"/>
         <v>24.88</v>
       </c>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D38" s="1">
+        <v>22.34</v>
+      </c>
+      <c r="E38" s="1">
         <v>21.46</v>
       </c>
-      <c r="E38" s="1">
+      <c r="F38" s="1">
         <v>92.77</v>
       </c>
-      <c r="F38" s="1">
+      <c r="G38" s="1">
         <v>70.349999999999994</v>
       </c>
-      <c r="G38" s="1">
+      <c r="H38" s="1">
         <v>76.8</v>
       </c>
-      <c r="H38" s="2">
+      <c r="I38" s="2">
         <v>34.14</v>
       </c>
-      <c r="I38" s="2">
+      <c r="J38" s="2">
         <f t="shared" si="1"/>
         <v>29.29</v>
       </c>
     </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D39" s="1">
+        <v>8.76</v>
+      </c>
+      <c r="E39" s="1">
         <v>4.97</v>
       </c>
-      <c r="E39" s="1">
+      <c r="F39" s="1">
         <v>91.92</v>
       </c>
-      <c r="F39" s="1">
+      <c r="G39" s="1">
         <v>62.41</v>
       </c>
-      <c r="G39" s="1">
+      <c r="H39" s="1">
         <v>78.09</v>
       </c>
-      <c r="H39" s="1">
+      <c r="I39" s="1">
         <v>35.58</v>
       </c>
-      <c r="I39" s="1">
+      <c r="J39" s="1">
         <f t="shared" si="1"/>
         <v>28.11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="C22:I22"/>
+  <mergeCells count="14">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:H23"/>
     <mergeCell ref="I23:I24"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="J3:J4"/>
     <mergeCell ref="D3:D4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="C23:C24"/>
     <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added size on disk
</commit_message>
<xml_diff>
--- a/eval_results_combined.xlsx
+++ b/eval_results_combined.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Thesis_Git\Complex-YOLOv3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5987F7B4-15D7-407A-B78F-B7449785038E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC2ADDF-021A-49B9-A0E5-A195A012F920}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{33803897-E998-4B3C-BE2B-F40B7580F66B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{33803897-E998-4B3C-BE2B-F40B7580F66B}"/>
   </bookViews>
   <sheets>
     <sheet name="Kitti" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="30">
   <si>
     <t>Model</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Size on disk (MB)</t>
   </si>
 </sst>
 </file>
@@ -144,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -167,15 +170,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -188,6 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,74 +520,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DCF2CE-8D1A-4C95-B84A-DAFE67D6BD13}">
-  <dimension ref="C2:J39"/>
+  <dimension ref="C2:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C2" s="4" t="s">
+    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="5" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="5" t="s">
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="1" t="s">
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
@@ -580,23 +605,26 @@
         <v>62.5</v>
       </c>
       <c r="F5" s="1">
+        <v>240.7</v>
+      </c>
+      <c r="G5" s="1">
         <v>93.59</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>70.44</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>86.39</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>658.12</v>
       </c>
-      <c r="J5" s="1">
-        <f>ROUND((1/I5)*1000,2)</f>
+      <c r="K5" s="1">
+        <f>ROUND((1/J5)*1000,2)</f>
         <v>1.52</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
@@ -607,23 +635,26 @@
         <v>12.5</v>
       </c>
       <c r="F6" s="1">
+        <v>47.8</v>
+      </c>
+      <c r="G6" s="1">
         <v>92.31</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>67.88</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>86.41</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>288.68</v>
       </c>
-      <c r="J6" s="1">
-        <f t="shared" ref="J6:J19" si="0">ROUND((1/I6)*1000,2)</f>
+      <c r="K6" s="1">
+        <f t="shared" ref="K6:K19" si="0">ROUND((1/J6)*1000,2)</f>
         <v>3.46</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
@@ -634,23 +665,26 @@
         <v>24.2</v>
       </c>
       <c r="F7" s="1">
+        <v>94.7</v>
+      </c>
+      <c r="G7" s="1">
         <v>89.93</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>72.7</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>79.41</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>297.18</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <f t="shared" si="0"/>
         <v>3.36</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
@@ -661,23 +695,26 @@
         <v>16.03</v>
       </c>
       <c r="F8" s="1">
+        <v>63</v>
+      </c>
+      <c r="G8" s="1">
         <v>75.95</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>54.74</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>74.239999999999995</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>271.89</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <f t="shared" si="0"/>
         <v>3.68</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
@@ -688,23 +725,26 @@
         <v>15.61</v>
       </c>
       <c r="F9" s="1">
+        <v>61.4</v>
+      </c>
+      <c r="G9" s="1">
         <v>85.07</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>48.89</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>56.21</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>290.02</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <f t="shared" si="0"/>
         <v>3.45</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
@@ -715,23 +755,26 @@
         <v>13.91</v>
       </c>
       <c r="F10" s="1">
+        <v>54.7</v>
+      </c>
+      <c r="G10" s="1">
         <v>91.56</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>59.76</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>80.98</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <v>220.02</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <f t="shared" si="0"/>
         <v>4.55</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
@@ -742,23 +785,26 @@
         <v>8.4700000000000006</v>
       </c>
       <c r="F11" s="1">
+        <v>33.4</v>
+      </c>
+      <c r="G11" s="1">
         <v>90.07</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <v>59.39</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>78.17</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>189.2</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <f t="shared" si="0"/>
         <v>5.29</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
@@ -769,23 +815,26 @@
         <v>5.7</v>
       </c>
       <c r="F12" s="1">
+        <v>22.5</v>
+      </c>
+      <c r="G12" s="1">
         <v>87.33</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>61.99</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>63.59</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <v>143.62</v>
       </c>
-      <c r="J12" s="2">
+      <c r="K12" s="2">
         <f t="shared" si="0"/>
         <v>6.96</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
@@ -796,23 +845,26 @@
         <v>7.79</v>
       </c>
       <c r="F13" s="1">
+        <v>30.7</v>
+      </c>
+      <c r="G13" s="1">
         <v>85.7</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>59.76</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>77.8</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>163.30000000000001</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K13" s="1">
         <f t="shared" si="0"/>
         <v>6.12</v>
       </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
@@ -823,23 +875,26 @@
         <v>7.79</v>
       </c>
       <c r="F14" s="1">
+        <v>30.7</v>
+      </c>
+      <c r="G14" s="1">
         <v>83.82</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>51.95</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>62.35</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <v>185.37</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K14" s="1">
         <f t="shared" si="0"/>
         <v>5.39</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
@@ -849,24 +904,27 @@
       <c r="E15" s="1">
         <v>22.13</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
+        <v>86.7</v>
+      </c>
+      <c r="G15" s="2">
         <v>92.59</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>70.28</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>83.09</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <v>272.52</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K15" s="1">
         <f t="shared" si="0"/>
         <v>3.67</v>
       </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>18</v>
       </c>
@@ -876,24 +934,27 @@
       <c r="E16" s="1">
         <v>22.12</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="9">
+        <v>86.65</v>
+      </c>
+      <c r="G16" s="1">
         <v>91.35</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <v>68.47</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>83.39</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <v>422.62</v>
       </c>
-      <c r="J16" s="1">
+      <c r="K16" s="1">
         <f t="shared" si="0"/>
         <v>2.37</v>
       </c>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>19</v>
       </c>
@@ -904,23 +965,26 @@
         <v>5.64</v>
       </c>
       <c r="F17" s="1">
+        <v>22.3</v>
+      </c>
+      <c r="G17" s="1">
         <v>85.07</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <v>66.150000000000006</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>79.92</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17" s="1">
         <v>308.04000000000002</v>
       </c>
-      <c r="J17" s="1">
+      <c r="K17" s="1">
         <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>20</v>
       </c>
@@ -931,23 +995,26 @@
         <v>21.46</v>
       </c>
       <c r="F18" s="1">
+        <v>84</v>
+      </c>
+      <c r="G18" s="1">
         <v>92.77</v>
       </c>
-      <c r="G18" s="3">
+      <c r="H18" s="3">
         <v>70.349999999999994</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>76.8</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J18" s="1">
         <v>289.95</v>
       </c>
-      <c r="J18" s="1">
+      <c r="K18" s="1">
         <f t="shared" si="0"/>
         <v>3.45</v>
       </c>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>21</v>
       </c>
@@ -957,74 +1024,80 @@
       <c r="E19" s="2">
         <v>4.97</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="2">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="G19" s="1">
         <v>91.92</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>62.41</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>78.09</v>
       </c>
-      <c r="I19" s="3">
+      <c r="J19" s="3">
         <v>182.67</v>
       </c>
-      <c r="J19" s="1">
+      <c r="K19" s="1">
         <f t="shared" si="0"/>
         <v>5.47</v>
       </c>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C22" s="4" t="s">
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="5" t="s">
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="4"/>
+      <c r="G23" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="5" t="s">
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="K23" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="1" t="s">
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>6</v>
       </c>
@@ -1034,24 +1107,25 @@
       <c r="E25" s="1">
         <v>62.5</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="1"/>
+      <c r="G25" s="1">
         <v>93.59</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <v>70.44</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <v>86.39</v>
       </c>
-      <c r="I25" s="1">
+      <c r="J25" s="1">
         <v>46.56</v>
       </c>
-      <c r="J25" s="1">
-        <f t="shared" ref="J25:J39" si="1">ROUND((1/I25)*1000,2)</f>
+      <c r="K25" s="1">
+        <f t="shared" ref="K25:K39" si="1">ROUND((1/J25)*1000,2)</f>
         <v>21.48</v>
       </c>
     </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>8</v>
       </c>
@@ -1061,24 +1135,25 @@
       <c r="E26" s="1">
         <v>12.5</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="1"/>
+      <c r="G26" s="1">
         <v>92.31</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <v>67.88</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="2">
         <v>86.41</v>
       </c>
-      <c r="I26" s="1">
+      <c r="J26" s="1">
         <v>34.64</v>
       </c>
-      <c r="J26" s="1">
+      <c r="K26" s="1">
         <f t="shared" si="1"/>
         <v>28.87</v>
       </c>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
         <v>9</v>
       </c>
@@ -1088,24 +1163,25 @@
       <c r="E27" s="1">
         <v>24.2</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="1"/>
+      <c r="G27" s="1">
         <v>89.93</v>
       </c>
-      <c r="G27" s="1">
+      <c r="H27" s="2">
         <v>72.7</v>
       </c>
-      <c r="H27" s="1">
+      <c r="I27" s="1">
         <v>79.41</v>
       </c>
-      <c r="I27" s="1">
+      <c r="J27" s="1">
         <v>45.02</v>
       </c>
-      <c r="J27" s="1">
+      <c r="K27" s="1">
         <f t="shared" si="1"/>
         <v>22.21</v>
       </c>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
         <v>10</v>
       </c>
@@ -1115,24 +1191,25 @@
       <c r="E28" s="1">
         <v>16.03</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="1"/>
+      <c r="G28" s="1">
         <v>75.95</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <v>54.74</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>74.239999999999995</v>
       </c>
-      <c r="I28" s="1">
+      <c r="J28" s="1">
         <v>37.57</v>
       </c>
-      <c r="J28" s="1">
+      <c r="K28" s="1">
         <f t="shared" si="1"/>
         <v>26.62</v>
       </c>
     </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>11</v>
       </c>
@@ -1142,24 +1219,25 @@
       <c r="E29" s="1">
         <v>15.61</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="1"/>
+      <c r="G29" s="1">
         <v>85.07</v>
       </c>
-      <c r="G29" s="1">
+      <c r="H29" s="1">
         <v>48.89</v>
       </c>
-      <c r="H29" s="1">
+      <c r="I29" s="1">
         <v>56.21</v>
       </c>
-      <c r="I29" s="1">
+      <c r="J29" s="1">
         <v>64.94</v>
       </c>
-      <c r="J29" s="1">
+      <c r="K29" s="1">
         <f t="shared" si="1"/>
         <v>15.4</v>
       </c>
     </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
         <v>12</v>
       </c>
@@ -1169,24 +1247,25 @@
       <c r="E30" s="1">
         <v>13.91</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="1"/>
+      <c r="G30" s="1">
         <v>91.56</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
         <v>59.76</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>80.98</v>
       </c>
-      <c r="I30" s="1">
+      <c r="J30" s="1">
         <v>38.31</v>
       </c>
-      <c r="J30" s="1">
+      <c r="K30" s="1">
         <f t="shared" si="1"/>
         <v>26.1</v>
       </c>
     </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
         <v>13</v>
       </c>
@@ -1196,24 +1275,25 @@
       <c r="E31" s="1">
         <v>8.4700000000000006</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31" s="1"/>
+      <c r="G31" s="1">
         <v>90.07</v>
       </c>
-      <c r="G31" s="1">
+      <c r="H31" s="1">
         <v>59.39</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <v>78.17</v>
       </c>
-      <c r="I31" s="1">
+      <c r="J31" s="1">
         <v>41.37</v>
       </c>
-      <c r="J31" s="1">
+      <c r="K31" s="1">
         <f t="shared" si="1"/>
         <v>24.17</v>
       </c>
     </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="1" t="s">
         <v>14</v>
       </c>
@@ -1223,24 +1303,25 @@
       <c r="E32" s="1">
         <v>5.7</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="1"/>
+      <c r="G32" s="1">
         <v>87.33</v>
       </c>
-      <c r="G32" s="1">
+      <c r="H32" s="1">
         <v>61.99</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <v>63.59</v>
       </c>
-      <c r="I32" s="1">
+      <c r="J32" s="1">
         <v>37.24</v>
       </c>
-      <c r="J32" s="1">
+      <c r="K32" s="1">
         <f t="shared" si="1"/>
         <v>26.85</v>
       </c>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
         <v>15</v>
       </c>
@@ -1250,24 +1331,25 @@
       <c r="E33" s="1">
         <v>7.79</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="1"/>
+      <c r="G33" s="1">
         <v>85.7</v>
       </c>
-      <c r="G33" s="1">
+      <c r="H33" s="1">
         <v>59.76</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <v>77.8</v>
       </c>
-      <c r="I33" s="1">
+      <c r="J33" s="1">
         <v>35.6</v>
       </c>
-      <c r="J33" s="1">
+      <c r="K33" s="1">
         <f t="shared" si="1"/>
         <v>28.09</v>
       </c>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>16</v>
       </c>
@@ -1277,24 +1359,25 @@
       <c r="E34" s="1">
         <v>7.79</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="1"/>
+      <c r="G34" s="1">
         <v>83.82</v>
       </c>
-      <c r="G34" s="1">
+      <c r="H34" s="1">
         <v>51.95</v>
       </c>
-      <c r="H34" s="1">
+      <c r="I34" s="1">
         <v>62.35</v>
       </c>
-      <c r="I34" s="1">
+      <c r="J34" s="1">
         <v>50.77</v>
       </c>
-      <c r="J34" s="1">
+      <c r="K34" s="1">
         <f t="shared" si="1"/>
         <v>19.7</v>
       </c>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
         <v>17</v>
       </c>
@@ -1304,24 +1387,25 @@
       <c r="E35" s="1">
         <v>22.13</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F35" s="1"/>
+      <c r="G35" s="2">
         <v>92.59</v>
       </c>
-      <c r="G35" s="1">
+      <c r="H35" s="1">
         <v>70.28</v>
       </c>
-      <c r="H35" s="1">
+      <c r="I35" s="1">
         <v>83.09</v>
       </c>
-      <c r="I35" s="1">
+      <c r="J35" s="1">
         <v>35.75</v>
       </c>
-      <c r="J35" s="1">
+      <c r="K35" s="1">
         <f t="shared" si="1"/>
         <v>27.97</v>
       </c>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>18</v>
       </c>
@@ -1331,24 +1415,25 @@
       <c r="E36" s="1">
         <v>22.12</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F36" s="1"/>
+      <c r="G36" s="1">
         <v>91.35</v>
       </c>
-      <c r="G36" s="1">
+      <c r="H36" s="1">
         <v>68.47</v>
       </c>
-      <c r="H36" s="1">
+      <c r="I36" s="1">
         <v>83.39</v>
       </c>
-      <c r="I36" s="1">
+      <c r="J36" s="1">
         <v>37.5</v>
       </c>
-      <c r="J36" s="1">
+      <c r="K36" s="1">
         <f t="shared" si="1"/>
         <v>26.67</v>
       </c>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
         <v>19</v>
       </c>
@@ -1358,24 +1443,25 @@
       <c r="E37" s="1">
         <v>5.64</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F37" s="1"/>
+      <c r="G37" s="1">
         <v>85.07</v>
       </c>
-      <c r="G37" s="1">
+      <c r="H37" s="1">
         <v>66.150000000000006</v>
       </c>
-      <c r="H37" s="1">
+      <c r="I37" s="1">
         <v>79.92</v>
       </c>
-      <c r="I37" s="1">
+      <c r="J37" s="1">
         <v>40.19</v>
       </c>
-      <c r="J37" s="1">
+      <c r="K37" s="1">
         <f t="shared" si="1"/>
         <v>24.88</v>
       </c>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
         <v>20</v>
       </c>
@@ -1385,66 +1471,69 @@
       <c r="E38" s="1">
         <v>21.46</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F38" s="1"/>
+      <c r="G38" s="1">
         <v>92.77</v>
       </c>
-      <c r="G38" s="1">
+      <c r="H38" s="1">
         <v>70.349999999999994</v>
       </c>
-      <c r="H38" s="1">
+      <c r="I38" s="1">
         <v>76.8</v>
       </c>
-      <c r="I38" s="2">
+      <c r="J38" s="2">
         <v>34.14</v>
       </c>
-      <c r="J38" s="2">
+      <c r="K38" s="2">
         <f t="shared" si="1"/>
         <v>29.29</v>
       </c>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D39" s="1">
         <v>8.76</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="2">
         <v>4.97</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F39" s="2"/>
+      <c r="G39" s="1">
         <v>91.92</v>
       </c>
-      <c r="G39" s="1">
+      <c r="H39" s="1">
         <v>62.41</v>
       </c>
-      <c r="H39" s="1">
+      <c r="I39" s="1">
         <v>78.09</v>
       </c>
-      <c r="I39" s="1">
+      <c r="J39" s="1">
         <v>35.58</v>
       </c>
-      <c r="J39" s="1">
+      <c r="K39" s="1">
         <f t="shared" si="1"/>
         <v>28.11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C22:J22"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="F3:H3"/>
+  <mergeCells count="15">
+    <mergeCell ref="C2:K2"/>
+    <mergeCell ref="C22:K22"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="G3:I3"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="E3:E4"/>
-    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="K3:K4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="D23:D24"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1471,52 +1560,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
       <c r="J2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="8"/>
       <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">

</xml_diff>

<commit_message>
Added size on disk for each model
</commit_message>
<xml_diff>
--- a/eval_results_combined.xlsx
+++ b/eval_results_combined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Thesis_Git\Complex-YOLOv3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC2ADDF-021A-49B9-A0E5-A195A012F920}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0B2210-3D80-4B72-87EE-0E98A37F3CC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{33803897-E998-4B3C-BE2B-F40B7580F66B}"/>
   </bookViews>
@@ -193,6 +193,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -205,7 +206,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,7 +523,7 @@
   <dimension ref="C2:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,48 +540,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="6" t="s">
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
       <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
@@ -591,8 +591,8 @@
       <c r="I4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
@@ -934,7 +934,7 @@
       <c r="E16" s="1">
         <v>22.12</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="5">
         <v>86.65</v>
       </c>
       <c r="G16" s="1">
@@ -1045,45 +1045,45 @@
       </c>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="4"/>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="6" t="s">
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K23" s="6" t="s">
+      <c r="K23" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="8"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="4"/>
       <c r="G24" s="1" t="s">
         <v>3</v>
@@ -1094,8 +1094,8 @@
       <c r="I24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
@@ -1560,52 +1560,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
       <c r="J2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="6" t="s">
+      <c r="F3" s="8"/>
+      <c r="G3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="8"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="9"/>
       <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">

</xml_diff>